<commit_message>
Runmode mode functionality added
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata3.xlsx
+++ b/src/test/resources/excel/testdata3.xlsx
@@ -4,54 +4,31 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="test_suite" sheetId="1" r:id="rId1"/>
-    <sheet name="LoginTest" sheetId="4" r:id="rId2"/>
-    <sheet name="CreateAccountTest" sheetId="5" r:id="rId3"/>
+    <sheet name="findNewCar" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
-    <t>TCID</t>
+    <t>browser</t>
   </si>
   <si>
-    <t>Runmode</t>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
   <si>
     <t>Y</t>
   </si>
   <si>
-    <t>runmode</t>
-  </si>
-  <si>
-    <t>LoginTest</t>
-  </si>
-  <si>
-    <t>username</t>
-  </si>
-  <si>
-    <t>password</t>
-  </si>
-  <si>
-    <t>gauravchauhan200@gmail.com</t>
-  </si>
-  <si>
-    <t>wpQ76sA4Ri@PNn2</t>
-  </si>
-  <si>
-    <t>CreateAccountTest</t>
-  </si>
-  <si>
-    <t>accountname</t>
-  </si>
-  <si>
-    <t>Raman</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -390,16 +367,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -407,94 +384,31 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="27.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
second test case initiated
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata3.xlsx
+++ b/src/test/resources/excel/testdata3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="31">
   <si>
     <t>browser</t>
   </si>
@@ -29,16 +29,101 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>carBrand</t>
+  </si>
+  <si>
+    <t>Hyundai</t>
+  </si>
+  <si>
+    <t>BMW</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Tata</t>
+  </si>
+  <si>
+    <t>Maruti Suzuki</t>
+  </si>
+  <si>
+    <t>Mahindra</t>
+  </si>
+  <si>
+    <t>Kia</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz</t>
+  </si>
+  <si>
+    <t>Honda</t>
+  </si>
+  <si>
+    <t>Skoda</t>
+  </si>
+  <si>
+    <t>MG</t>
+  </si>
+  <si>
+    <t>carTitle</t>
+  </si>
+  <si>
+    <t>Maruti Suzuki Cars</t>
+  </si>
+  <si>
+    <t>Hyundai Cars</t>
+  </si>
+  <si>
+    <t>Tata Cars</t>
+  </si>
+  <si>
+    <t>Mahindra Cars</t>
+  </si>
+  <si>
+    <t>Kia Cars</t>
+  </si>
+  <si>
+    <t>Toyota Cars</t>
+  </si>
+  <si>
+    <t>Volkswagen Cars</t>
+  </si>
+  <si>
+    <t>Mercedes-Benz Cars</t>
+  </si>
+  <si>
+    <t>Honda Cars</t>
+  </si>
+  <si>
+    <t>Volkswagen</t>
+  </si>
+  <si>
+    <t>Skoda Cars</t>
+  </si>
+  <si>
+    <t>BMW Cars</t>
+  </si>
+  <si>
+    <t>MG Cars</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF202124"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -64,8 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -367,51 +453,204 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.7109375" customWidth="1"/>
-    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="2" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
suite and excel run mode updated
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testdata3.xlsx
+++ b/src/test/resources/excel/testdata3.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="findNewCar" sheetId="1" r:id="rId1"/>
@@ -456,8 +456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -493,7 +493,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -507,7 +507,7 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -535,7 +535,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -549,7 +549,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -563,7 +563,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -577,7 +577,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -591,7 +591,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -605,7 +605,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -619,7 +619,7 @@
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -633,7 +633,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,7 +647,7 @@
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -660,7 +660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -696,7 +696,7 @@
         <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -738,7 +738,7 @@
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -752,7 +752,7 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -766,7 +766,7 @@
         <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -794,7 +794,7 @@
         <v>25</v>
       </c>
       <c r="D9" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -808,7 +808,7 @@
         <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -822,7 +822,7 @@
         <v>28</v>
       </c>
       <c r="D11" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -836,7 +836,7 @@
         <v>29</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -850,7 +850,7 @@
         <v>30</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>